<commit_message>
not db yet, but made a bunch of other improvements
</commit_message>
<xml_diff>
--- a/stock_template.xlsx
+++ b/stock_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamiller1\Desktop\copyroom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cadb858e6df91a75/repo/copy_room_inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02504128-9C3F-4C05-AE74-50B63890BCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{A6EE2A98-C989-44DE-9FBB-6637E597FF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABAEBCA0-12C6-4F0E-A92C-50AB95D9FC9F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="checkouts" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
   <si>
     <t>item_id</t>
   </si>
@@ -231,13 +231,25 @@
     <t>single</t>
   </si>
   <si>
-    <t>school</t>
-  </si>
-  <si>
     <t>Fremont</t>
   </si>
   <si>
-    <t>email</t>
+    <t>background_link</t>
+  </si>
+  <si>
+    <t>School Name</t>
+  </si>
+  <si>
+    <t>users_name</t>
+  </si>
+  <si>
+    <t>Karrie</t>
+  </si>
+  <si>
+    <t>https://static.vecteezy.com/system/resources/previews/038/035/644/large_2x/ai-generated-wolf-high-quality-image-free-photo.jpg</t>
+  </si>
+  <si>
+    <t>buffer_amount</t>
   </si>
 </sst>
 </file>
@@ -247,7 +259,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +292,12 @@
       <b/>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -327,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -339,6 +357,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -684,9 +704,9 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -725,19 +745,19 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.25" customWidth="1"/>
-    <col min="4" max="4" width="10.9140625" customWidth="1"/>
+    <col min="1" max="1" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.9140625" customWidth="1"/>
-    <col min="9" max="9" width="70.4140625" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" customWidth="1"/>
+    <col min="9" max="9" width="70.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -766,7 +786,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>31</v>
       </c>
@@ -795,7 +815,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>32</v>
       </c>
@@ -806,7 +826,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>24</v>
       </c>
@@ -832,7 +852,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>22</v>
       </c>
@@ -858,7 +878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>16</v>
       </c>
@@ -884,7 +904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>35</v>
       </c>
@@ -913,7 +933,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>17</v>
       </c>
@@ -942,7 +962,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>12</v>
       </c>
@@ -968,7 +988,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -991,7 +1011,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1014,7 +1034,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1055,13 +1075,13 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1075,7 +1095,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -1089,7 +1109,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -1103,7 +1123,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -1117,7 +1137,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -1131,7 +1151,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -1145,7 +1165,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -1159,7 +1179,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -1173,7 +1193,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -1187,7 +1207,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -1201,7 +1221,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1010</v>
       </c>
@@ -1215,7 +1235,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1011</v>
       </c>
@@ -1229,7 +1249,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1012</v>
       </c>
@@ -1243,7 +1263,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1013</v>
       </c>
@@ -1257,7 +1277,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1014</v>
       </c>
@@ -1271,7 +1291,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1015</v>
       </c>
@@ -1298,13 +1318,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="10.9140625" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1312,7 +1332,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1320,7 +1340,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1328,7 +1348,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1349,14 +1369,14 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.58203125" customWidth="1"/>
-    <col min="2" max="2" width="47.08203125" customWidth="1"/>
-    <col min="3" max="3" width="37.75" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="47.109375" customWidth="1"/>
+    <col min="3" max="3" width="37.77734375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>30</v>
       </c>
@@ -1367,7 +1387,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1378,7 +1398,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1389,7 +1409,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1400,7 +1420,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1411,7 +1431,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1430,33 +1450,51 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0219849-C054-49EE-91B4-6C78C58B0825}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="42.44140625" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>69</v>
+      <c r="B2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="8">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{B1C69DCE-8611-49F8-9F2F-C6C7DC9565B7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>